<commit_message>
Inicio de la propuesta , falta requisitos
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="973" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -131,6 +131,102 @@
   </si>
   <si>
     <t xml:space="preserve">Difícil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Noticias </t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear una tabla donde se guardaran los datos de la noticia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Liga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear una tabla con los datos de cada liga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crea tabla Equipos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear una tabla con los datos de cada equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Jugadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear una tabla con los datos de cada jugador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crea tabla Partidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear una tabla con los datos de cada partido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generar Estadisticas jugadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener una lista con estadisticas de jugadores según sus partidos (goles,partidos jugados…)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener un buscador para acceder rapidamente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Posts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una tabla donde se almacenara los datos de cada entrada en el foro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Respuestas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una tabla donde se almacenara los datos de cada respuesta en el post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear herramienta de tacticas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una herramienta de diseño para la creacion de tacticas y estrategias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Img Predefinidas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una tabla para almacenar imagenes como plantilla para la herramienta de diseño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Img Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">una tabla para guardar las imagenes como plantilla para cada usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Equipo Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donde se almacenar los datos de los equipos de los usuarios para compartir sus tacticas de forma privada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear tabla Miembro Equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donde se guarda cada participante de cada equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear Tabla Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tabla que almacena los datos de cada usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear atajos de teclaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para acceder rapidamente a las distintas pestañas</t>
   </si>
 </sst>
 </file>
@@ -270,19 +366,19 @@
   </sheetPr>
   <dimension ref="A1:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B17" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="54.1326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -424,6 +520,134 @@
       </c>
       <c r="G6" s="8" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>